<commit_message>
Update code. fix issues
</commit_message>
<xml_diff>
--- a/anketa.xlsx
+++ b/anketa.xlsx
@@ -131,11 +131,12 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -171,12 +172,6 @@
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -293,7 +288,9 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -336,43 +333,43 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="3" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -456,23 +453,20 @@
   </sheetPr>
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P3" activeCellId="0" sqref="P3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA4" activeCellId="0" sqref="AA4:AE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.9296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="1" style="1" width="12.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.2"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="4" style="1" width="12.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="11" style="1" width="12.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="1" style="1" width="12.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="1" width="12.75"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="24" min="23" style="1" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="14.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="19.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="26.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="22.49"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="1" width="40.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="40.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="28.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="22.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="32" style="1" width="15.91"/>
@@ -613,6 +607,7 @@
     <row r="3" customFormat="false" ht="133.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -622,7 +617,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
-      <c r="M3" s="11"/>
+      <c r="M3" s="12"/>
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
       <c r="P3" s="9"/>
@@ -635,11 +630,12 @@
       <c r="W3" s="9"/>
       <c r="X3" s="9"/>
       <c r="Y3" s="9"/>
-      <c r="Z3" s="12"/>
-      <c r="AA3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="11"/>
       <c r="AC3" s="14"/>
       <c r="AD3" s="14"/>
-      <c r="AE3" s="13"/>
+      <c r="AE3" s="14"/>
     </row>
     <row r="4" customFormat="false" ht="69" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15"/>
@@ -669,6 +665,9 @@
       <c r="Y4" s="16"/>
       <c r="Z4" s="17"/>
       <c r="AA4" s="18"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
       <c r="AE4" s="14"/>
     </row>
     <row r="5" customFormat="false" ht="69" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>